<commit_message>
se crean clases nuevas de consolidacion
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/preApproved.xlsx
+++ b/src/test/resources/dataDriven/preApproved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bcs-credito-digital\src\test\resources\dataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF4F10F-AD3F-4588-9D55-59888BB6AF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A2D029-E8D9-4D3B-AB55-6F727E8BDC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
   </bookViews>
   <sheets>
     <sheet name="landing" sheetId="6" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="validateModal" sheetId="13" r:id="rId6"/>
     <sheet name="happyPath2E2" sheetId="4" r:id="rId7"/>
     <sheet name="accounts" sheetId="14" r:id="rId8"/>
+    <sheet name="consolidated" sheetId="17" r:id="rId9"/>
+    <sheet name="offer" sheetId="16" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
   <si>
     <t>idType</t>
   </si>
@@ -225,6 +227,15 @@
   </si>
   <si>
     <t>activar su cuenta</t>
+  </si>
+  <si>
+    <t>txtAccount</t>
+  </si>
+  <si>
+    <t>txtConsolidated</t>
+  </si>
+  <si>
+    <t>pendiente el pago</t>
   </si>
 </sst>
 </file>
@@ -612,6 +623,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE590A32-C60D-4428-AD64-8F85D7B76387}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>94387989</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252687B5-B7E8-43A1-A660-258C89852C6D}">
   <dimension ref="A1:E2"/>
@@ -728,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CDF921E-921E-43FF-813E-46494BB1673C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +1088,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>10009287</v>
+        <v>33152814</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>49</v>
@@ -1260,7 +1353,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H2" sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,4 +1422,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42C6B4C-BAD6-4BDB-9E94-6C48097AB142}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>94387989</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se agregan los features que se van a usar mas adelante
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/preApproved.xlsx
+++ b/src/test/resources/dataDriven/preApproved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bcs-credito-digital\src\test\resources\dataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A2D029-E8D9-4D3B-AB55-6F727E8BDC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B677609-7B66-4AB6-AE41-21FA354B76EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
   </bookViews>
   <sheets>
     <sheet name="landing" sheetId="6" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="validationsMessages" sheetId="12" r:id="rId5"/>
     <sheet name="validateModal" sheetId="13" r:id="rId6"/>
     <sheet name="happyPath2E2" sheetId="4" r:id="rId7"/>
-    <sheet name="accounts" sheetId="14" r:id="rId8"/>
-    <sheet name="consolidated" sheetId="17" r:id="rId9"/>
-    <sheet name="offer" sheetId="16" r:id="rId10"/>
+    <sheet name="accounts" sheetId="18" r:id="rId8"/>
+    <sheet name="noAccounts" sheetId="14" r:id="rId9"/>
+    <sheet name="consolidated" sheetId="17" r:id="rId10"/>
+    <sheet name="offer" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="66">
   <si>
     <t>idType</t>
   </si>
@@ -236,6 +237,9 @@
   </si>
   <si>
     <t>pendiente el pago</t>
+  </si>
+  <si>
+    <t>txtBeneficiary</t>
   </si>
 </sst>
 </file>
@@ -624,11 +628,85 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42C6B4C-BAD6-4BDB-9E94-6C48097AB142}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>94387989</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE590A32-C60D-4428-AD64-8F85D7B76387}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>94387989</v>
+        <v>1013583153</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>49</v>
@@ -822,7 +900,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +908,7 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -872,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>94387989</v>
+        <v>1013583153</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>49</v>
@@ -1349,11 +1427,99 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBAACD0-1B59-413C-B1AA-5A3D3791604F}">
+  <dimension ref="B1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1013583153</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A30DB37-C5FE-4EE6-8412-F58989A7CDCE}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="A1:H2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,78 +1588,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42C6B4C-BAD6-4BDB-9E94-6C48097AB142}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>94387989</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
se agregan dependencia de rest assured
</commit_message>
<xml_diff>
--- a/src/test/resources/dataDriven/preApproved.xlsx
+++ b/src/test/resources/dataDriven/preApproved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bcs-credito-digital\src\test\resources\dataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B677609-7B66-4AB6-AE41-21FA354B76EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5ED8D6-DBA0-4078-B2A3-97676142363B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="5" activeTab="7" xr2:uid="{565A5E9C-6FFF-4ECB-8A93-B318EC1ABE36}"/>
   </bookViews>
   <sheets>
     <sheet name="landing" sheetId="6" r:id="rId1"/>
@@ -1431,7 +1431,7 @@
   <dimension ref="B1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>